<commit_message>
edit spreadsheet, add design doc
</commit_message>
<xml_diff>
--- a/docs/SurteesToby_Claims.xlsx
+++ b/docs/SurteesToby_Claims.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d1f6318edab0ffd/Documents/comp2013_cw/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{5EC6E55A-F6B8-4754-8C6D-7F31B666D0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6036C089-D6C1-46C9-9171-DDDAEF709E84}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{5EC6E55A-F6B8-4754-8C6D-7F31B666D0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C6F977D-3841-46BE-A555-364554598902}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,9 +158,6 @@
     <t>Converted project to use Maven, added all relevant dependancies.</t>
   </si>
   <si>
-    <t>No swing remains in the code.</t>
-  </si>
-  <si>
     <t>Filled out module-info file with correct information.</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bonus fruits, golden fruit adds 500, rotten fruit takes 100 away, dissapear after 5 seconds (SnakeFood Class). Walls to be avoided, change position and orientation every 5 seconds (SnakeWall Class). Can be disabled in settings (SettingsScene Class). Game over screen, has a place to enter a name to go on the leaderboard, previously mentioned buttons, a countdown from 10 that restarts the game. (gameOverScreen() method in SnakeView). A sleek pause menu when you press ESC in game, has volume slider and restart and main menu buttons. (pauseGame() unpauseGame() methods in SnakeView) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No swing remains in the code. All scenes are in View/SnakeScenes. The view is controlled by SnakeView which implementes IView. </t>
   </si>
 </sst>
 </file>
@@ -380,10 +380,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -752,7 +748,7 @@
         <v>36</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
@@ -763,7 +759,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -774,7 +770,7 @@
         <v>36</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -807,7 +803,7 @@
         <v>36</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -829,7 +825,7 @@
         <v>36</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -840,7 +836,7 @@
         <v>36</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="45" x14ac:dyDescent="0.25">
@@ -860,7 +856,7 @@
         <v>36</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -871,7 +867,7 @@
         <v>36</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -882,7 +878,7 @@
         <v>36</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -893,7 +889,7 @@
         <v>36</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -904,7 +900,7 @@
         <v>36</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -915,7 +911,7 @@
         <v>36</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:4" s="20" customFormat="1" ht="165" x14ac:dyDescent="0.25">
@@ -926,7 +922,7 @@
         <v>36</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>